<commit_message>
Tj and xij does not match
</commit_message>
<xml_diff>
--- a/Параметры модели (version 1).xlsb.xlsx
+++ b/Параметры модели (version 1).xlsb.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2039915D-F7B5-4435-A62B-664E36EB4F2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515FB56F-5DB1-4FD7-BE0D-E0DD21F594A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Свойства компонентов" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,9 @@
     <sheet name="Лист2" sheetId="6" r:id="rId6"/>
     <sheet name="teta" sheetId="7" r:id="rId7"/>
     <sheet name="Лист3" sheetId="8" r:id="rId8"/>
+    <sheet name="kij" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3059" uniqueCount="1934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3124" uniqueCount="1998">
   <si>
     <t>№</t>
   </si>
@@ -6473,6 +6473,198 @@
   <si>
     <t>391.663084445343</t>
   </si>
+  <si>
+    <t>kij</t>
+  </si>
+  <si>
+    <t>iC4</t>
+  </si>
+  <si>
+    <t>(328,15081705153,</t>
+  </si>
+  <si>
+    <t>328,321820214391,</t>
+  </si>
+  <si>
+    <t>345,370900034904,</t>
+  </si>
+  <si>
+    <t>367,08410564065,</t>
+  </si>
+  <si>
+    <t>385,682712197304,</t>
+  </si>
+  <si>
+    <t>398,748969011009,</t>
+  </si>
+  <si>
+    <t>405,961940616369,</t>
+  </si>
+  <si>
+    <t>406,08185184747,</t>
+  </si>
+  <si>
+    <t>397,916830688715,</t>
+  </si>
+  <si>
+    <t>383,789538115263,</t>
+  </si>
+  <si>
+    <t>425,514830768108,</t>
+  </si>
+  <si>
+    <t>438,657890416682,</t>
+  </si>
+  <si>
+    <t>441,55496352911,</t>
+  </si>
+  <si>
+    <t>442,359023191035,</t>
+  </si>
+  <si>
+    <t>442,699845634401,</t>
+  </si>
+  <si>
+    <t>442,886493049562,</t>
+  </si>
+  <si>
+    <t>442,989338867366,</t>
+  </si>
+  <si>
+    <t>443,027738198638,</t>
+  </si>
+  <si>
+    <t>443,001218631864,</t>
+  </si>
+  <si>
+    <t>442,887031815946,</t>
+  </si>
+  <si>
+    <t>442,612266816199,</t>
+  </si>
+  <si>
+    <t>441,922629654408,</t>
+  </si>
+  <si>
+    <t>450,02378360182,</t>
+  </si>
+  <si>
+    <t>450,645598076284,</t>
+  </si>
+  <si>
+    <t>450,001883886755,</t>
+  </si>
+  <si>
+    <t>449,111589789391,</t>
+  </si>
+  <si>
+    <t>448,144888274372,</t>
+  </si>
+  <si>
+    <t>447,150192454457,</t>
+  </si>
+  <si>
+    <t>446,161065228283,</t>
+  </si>
+  <si>
+    <t>445,209517866373,</t>
+  </si>
+  <si>
+    <t>444,325442649424,</t>
+  </si>
+  <si>
+    <t>443,534251943231,</t>
+  </si>
+  <si>
+    <t>442,855051346123,</t>
+  </si>
+  <si>
+    <t>442,299723751843,</t>
+  </si>
+  <si>
+    <t>441,873084127903,</t>
+  </si>
+  <si>
+    <t>441,573760688305,</t>
+  </si>
+  <si>
+    <t>441,39555567503,</t>
+  </si>
+  <si>
+    <t>441,3289244771,</t>
+  </si>
+  <si>
+    <t>441,362406551838,</t>
+  </si>
+  <si>
+    <t>441,4839630723,</t>
+  </si>
+  <si>
+    <t>441,682162702084,</t>
+  </si>
+  <si>
+    <t>441,947297275066,</t>
+  </si>
+  <si>
+    <t>442,272404782474,</t>
+  </si>
+  <si>
+    <t>442,65424374491,</t>
+  </si>
+  <si>
+    <t>443,093969598413,</t>
+  </si>
+  <si>
+    <t>443,59754781425,</t>
+  </si>
+  <si>
+    <t>444,175597913563,</t>
+  </si>
+  <si>
+    <t>444,842559434474,</t>
+  </si>
+  <si>
+    <t>445,614942342043,</t>
+  </si>
+  <si>
+    <t>446,508663512766,</t>
+  </si>
+  <si>
+    <t>447,535371169448,</t>
+  </si>
+  <si>
+    <t>448,69850345701,</t>
+  </si>
+  <si>
+    <t>449,990072846413,</t>
+  </si>
+  <si>
+    <t>451,389738574624,</t>
+  </si>
+  <si>
+    <t>452,86747495085,</t>
+  </si>
+  <si>
+    <t>454,38980717212,</t>
+  </si>
+  <si>
+    <t>455,928384646773,</t>
+  </si>
+  <si>
+    <t>457,468712508678,</t>
+  </si>
+  <si>
+    <t>459,018961712718,</t>
+  </si>
+  <si>
+    <t>460,627420447767,</t>
+  </si>
+  <si>
+    <t>462,480454929173,</t>
+  </si>
+  <si>
+    <t>465,829186677933)</t>
+  </si>
 </sst>
 </file>
 
@@ -6482,12 +6674,20 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6551,6 +6751,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -6595,49 +6802,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="2" xr:uid="{AFF3F87A-FDE4-4506-86B2-2B9AE26B9163}"/>
+    <cellStyle name="Обычный 3" xfId="1" xr:uid="{460BCC82-989A-4065-9474-79ABD5EFF6CE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -6901,190 +7113,190 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>-58.205179707705952</c:v>
+                  <c:v>55.000817051530021</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58.626986457407497</c:v>
+                  <c:v>55.171820214391005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.081676228344463</c:v>
+                  <c:v>72.220900034904048</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108.71960984021428</c:v>
+                  <c:v>93.934105640650046</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122.88854920715096</c:v>
+                  <c:v>112.53271219730402</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128.84751611799004</c:v>
+                  <c:v>125.59896901100905</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>132.0132655784488</c:v>
+                  <c:v>132.81194061636904</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>135.05399541407826</c:v>
+                  <c:v>132.93185184747</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>138.50626849979164</c:v>
+                  <c:v>124.766830688715</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>141.76056587547066</c:v>
+                  <c:v>110.63953811526301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>151.79324352592232</c:v>
+                  <c:v>152.36483076810805</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>153.29639853388073</c:v>
+                  <c:v>165.50789041668202</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>153.63409274667504</c:v>
+                  <c:v>168.40496352911003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>153.80268969982865</c:v>
+                  <c:v>169.20902319103504</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>153.93933036774399</c:v>
+                  <c:v>169.54984563440104</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>154.06756715327504</c:v>
+                  <c:v>169.736493049562</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>154.19370771795514</c:v>
+                  <c:v>169.839338867366</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>154.32059557586911</c:v>
+                  <c:v>169.87773819863804</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>154.45014329105618</c:v>
+                  <c:v>169.85121863186401</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>154.58409243673088</c:v>
+                  <c:v>169.73703181594601</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>154.72448856979611</c:v>
+                  <c:v>169.46226681619902</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>154.87401054650547</c:v>
+                  <c:v>168.77262965440804</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>155.05002343505623</c:v>
+                  <c:v>176.87378360182004</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>155.22905082851651</c:v>
+                  <c:v>177.49559807628401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>155.42475299388173</c:v>
+                  <c:v>176.85188388675505</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>155.64350092262032</c:v>
+                  <c:v>175.96158978939104</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>155.89207091778519</c:v>
+                  <c:v>174.99488827437204</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>156.17892385870221</c:v>
+                  <c:v>174.00019245445702</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>156.51470550745728</c:v>
+                  <c:v>173.01106522828303</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>156.9126138225198</c:v>
+                  <c:v>172.05951786637303</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>157.38863327950241</c:v>
+                  <c:v>171.17544264942404</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>157.9614398762584</c:v>
+                  <c:v>170.38425194323105</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>158.65193249136212</c:v>
+                  <c:v>169.70505134612301</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>159.48194095343354</c:v>
+                  <c:v>169.149723751843</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>160.47199049443009</c:v>
+                  <c:v>168.72308412790301</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>161.63801492601635</c:v>
+                  <c:v>168.42376068830504</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>162.98725285977127</c:v>
+                  <c:v>168.24555567503</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>164.51408059746029</c:v>
+                  <c:v>168.1789244771</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>166.19709262102845</c:v>
+                  <c:v>168.212406551838</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>167.99874694496395</c:v>
+                  <c:v>168.33396307230004</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>169.86855694502594</c:v>
+                  <c:v>168.53216270208401</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>171.74947501569989</c:v>
+                  <c:v>168.797297275066</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>173.58582147806885</c:v>
+                  <c:v>169.12240478247401</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>175.33059285432103</c:v>
+                  <c:v>169.50424374491001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>176.95013561695816</c:v>
+                  <c:v>169.94396959841305</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>178.42553944736721</c:v>
+                  <c:v>170.44754781425002</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>179.75121231228115</c:v>
+                  <c:v>171.02559791356305</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>180.93176463097336</c:v>
+                  <c:v>171.69255943447405</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>181.97841213494542</c:v>
+                  <c:v>172.464942342043</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>182.90577137321236</c:v>
+                  <c:v>173.35866351276604</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>183.72949117273095</c:v>
+                  <c:v>174.38537116944804</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>184.46491637676957</c:v>
+                  <c:v>175.54850345701004</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>185.12687252312901</c:v>
+                  <c:v>176.84007284641302</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>185.73079311698677</c:v>
+                  <c:v>178.23973857462403</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>186.29528449326756</c:v>
+                  <c:v>179.71747495085003</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>186.8454189732671</c:v>
+                  <c:v>181.23980717212004</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>187.41488174945118</c:v>
+                  <c:v>182.77838464677302</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>188.04459662586453</c:v>
+                  <c:v>184.318712508678</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>188.78096544593575</c:v>
+                  <c:v>185.86896171271803</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>189.68890772610905</c:v>
+                  <c:v>187.47742044776703</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>190.95411316901448</c:v>
+                  <c:v>189.33045492917302</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>193.82552409023049</c:v>
+                  <c:v>192.67918667793305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8308,190 +8520,190 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>376.20000126596278</c:v>
+                  <c:v>376.19999867213244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>867.9917455829675</c:v>
+                  <c:v>909.85364381938552</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>722.82649187318975</c:v>
+                  <c:v>811.11426126007427</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>628.99995090415359</c:v>
+                  <c:v>712.45688666045044</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>589.31788134235785</c:v>
+                  <c:v>643.48412279106265</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>567.86493934369014</c:v>
+                  <c:v>614.88214315558139</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>545.68109523684029</c:v>
+                  <c:v>636.11191126241943</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>519.92449148269702</c:v>
+                  <c:v>702.61492060264573</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>498.32001842727118</c:v>
+                  <c:v>777.8852463783378</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2051.006183820733</c:v>
+                  <c:v>2089.2544696749046</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2055.5090818604285</c:v>
+                  <c:v>2045.3642735460312</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2056.2079786147524</c:v>
+                  <c:v>2048.9037162776849</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2056.4149139530045</c:v>
+                  <c:v>2049.471863946123</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2056.6640597590663</c:v>
+                  <c:v>2049.2217861181471</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2056.9776320920155</c:v>
+                  <c:v>2049.0606017975488</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2057.3343093744866</c:v>
+                  <c:v>2049.0901984861221</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2057.7176956350113</c:v>
+                  <c:v>2049.3124812701435</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2058.1175381047469</c:v>
+                  <c:v>2049.7661798812583</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2058.5272313851319</c:v>
+                  <c:v>2050.5828032628233</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2058.9416942055032</c:v>
+                  <c:v>2052.0927967116995</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2059.3557726827576</c:v>
+                  <c:v>2055.1880157777414</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2161.8725261154887</c:v>
+                  <c:v>2079.6829001349533</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2162.2685348627374</c:v>
+                  <c:v>2089.6522125134493</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2162.6320508319604</c:v>
+                  <c:v>2093.8347542120609</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2162.9619404110949</c:v>
+                  <c:v>2097.0369538259174</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2163.2447272041863</c:v>
+                  <c:v>2100.2131034368695</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2163.4599146675514</c:v>
+                  <c:v>2103.4616496155077</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2163.5790887565763</c:v>
+                  <c:v>2106.7410073133951</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2163.5641461400651</c:v>
+                  <c:v>2109.9837721712488</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2163.3655167382658</c:v>
+                  <c:v>2113.1175366562934</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2162.9209523929394</c:v>
+                  <c:v>2116.072703839036</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2162.1555640906658</c:v>
+                  <c:v>2118.7881680600103</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2160.9845294087968</c:v>
+                  <c:v>2121.2160497266177</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2159.3193346659336</c:v>
+                  <c:v>2123.3246214328178</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2157.0787096583044</c:v>
+                  <c:v>2125.0993461402313</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2154.204028405552</c:v>
+                  <c:v>2126.5417820348771</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2150.6769076461283</c:v>
+                  <c:v>2127.6669405904549</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2146.5343135290996</c:v>
+                  <c:v>2128.499532554295</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2141.8751890000103</c:v>
+                  <c:v>2129.0696848081507</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2136.8536352480724</c:v>
+                  <c:v>2129.4085592256206</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2131.6586199086041</c:v>
+                  <c:v>2129.5439550814513</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2126.4856340255246</c:v>
+                  <c:v>2129.4961499048677</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2121.5091542204245</c:v>
+                  <c:v>2129.2740977783824</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2116.8639076771515</c:v>
+                  <c:v>2128.8724620812809</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2112.6377433430371</c:v>
+                  <c:v>2128.2695938737802</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2108.8745424564959</c:v>
+                  <c:v>2127.4275086505199</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2105.582892299843</c:v>
+                  <c:v>2126.2944122376734</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2102.7463492180677</c:v>
+                  <c:v>2124.8110057568747</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2100.3327451973105</c:v>
+                  <c:v>2122.9214452876827</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2098.3017240356585</c:v>
+                  <c:v>2120.5895308067616</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2096.6109325394668</c:v>
+                  <c:v>2117.8181076003848</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2095.2221254933615</c:v>
+                  <c:v>2114.6676641757736</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2094.1085898184956</c:v>
+                  <c:v>2111.2666937369449</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2093.2646229523093</c:v>
+                  <c:v>2107.8070224674657</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2092.7147796982026</c:v>
+                  <c:v>2104.5222211951464</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2092.5159707604748</c:v>
+                  <c:v>2101.6545229242302</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2092.7464018747601</c:v>
+                  <c:v>2099.4215294762362</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2093.4842527739424</c:v>
+                  <c:v>2097.9903552770065</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2094.7762398134846</c:v>
+                  <c:v>2097.4494708708626</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2096.4866645703069</c:v>
+                  <c:v>2097.665771725543</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2097.3023796413254</c:v>
+                  <c:v>2097.3024261658516</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>408.09999558158256</c:v>
+                  <c:v>408.10000463447784</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9534,187 +9746,187 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1689.2000056843815</c:v>
+                  <c:v>1689.1999940376559</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2180.9917500013862</c:v>
+                  <c:v>2222.8536391849088</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2035.8264962916085</c:v>
+                  <c:v>2124.1142566255976</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1941.9999553225723</c:v>
+                  <c:v>2025.4568820259738</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1902.3178857607766</c:v>
+                  <c:v>1956.484118156586</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1880.8649437621089</c:v>
+                  <c:v>1927.8821385211047</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1858.681099655259</c:v>
+                  <c:v>1949.1119066279427</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1832.9244959011157</c:v>
+                  <c:v>2015.614915968169</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1811.3200228456899</c:v>
+                  <c:v>2090.8852417438611</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1746.0061882391517</c:v>
+                  <c:v>1784.2544650404282</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1750.5090862788472</c:v>
+                  <c:v>1740.3642689115545</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1751.2079830331709</c:v>
+                  <c:v>1743.9037116432082</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1751.414918371423</c:v>
+                  <c:v>1744.4718593116463</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1751.664064177485</c:v>
+                  <c:v>1744.2217814836706</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1751.9776365104342</c:v>
+                  <c:v>1744.0605971630719</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1752.3343137929053</c:v>
+                  <c:v>1744.0901938516452</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1752.71770005343</c:v>
+                  <c:v>1744.3124766356666</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1753.1175425231654</c:v>
+                  <c:v>1744.7661752467816</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1753.5272358035509</c:v>
+                  <c:v>1745.5827986283468</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1753.9416986239216</c:v>
+                  <c:v>1747.0927920772228</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1754.355777101176</c:v>
+                  <c:v>1750.1880111432645</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1753.7725305339075</c:v>
+                  <c:v>1671.5828955004765</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1754.1685392811562</c:v>
+                  <c:v>1681.5522078789725</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1754.5320552503792</c:v>
+                  <c:v>1685.7347495775841</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1754.8619448295135</c:v>
+                  <c:v>1688.9369491914406</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1755.1447316226049</c:v>
+                  <c:v>1692.1130988023929</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1755.35991908597</c:v>
+                  <c:v>1695.3616449810308</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1755.4790931749951</c:v>
+                  <c:v>1698.6410026789185</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1755.4641505584839</c:v>
+                  <c:v>1701.883767536772</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1755.2655211566846</c:v>
+                  <c:v>1705.0175320218166</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1754.820956811358</c:v>
+                  <c:v>1707.9726992045594</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1754.0555685090844</c:v>
+                  <c:v>1710.6881634255337</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1752.8845338272154</c:v>
+                  <c:v>1713.1160450921411</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1751.2193390843524</c:v>
+                  <c:v>1715.224616798341</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1748.978714076723</c:v>
+                  <c:v>1716.9993415057545</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1746.1040328239708</c:v>
+                  <c:v>1718.4417774004005</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1742.5769120645468</c:v>
+                  <c:v>1719.5669359559784</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1738.4343179475184</c:v>
+                  <c:v>1720.3995279198184</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1733.7751934184289</c:v>
+                  <c:v>1720.9696801736739</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1728.7536396664909</c:v>
+                  <c:v>1721.3085545911438</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1723.5586243270227</c:v>
+                  <c:v>1721.4439504469744</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1718.3856384439432</c:v>
+                  <c:v>1721.3961452703911</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1713.4091586388433</c:v>
+                  <c:v>1721.1740931439058</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1708.76391209557</c:v>
+                  <c:v>1720.7724574468043</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1704.5377477614559</c:v>
+                  <c:v>1720.1695892393034</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1700.7745468749144</c:v>
+                  <c:v>1719.3275040160433</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1697.4828967182616</c:v>
+                  <c:v>1718.1944076031969</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1694.6463536364865</c:v>
+                  <c:v>1716.7110011223981</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1692.2327496157293</c:v>
+                  <c:v>1714.8214406532059</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1690.2017284540771</c:v>
+                  <c:v>1712.4895261722847</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1688.5109369578856</c:v>
+                  <c:v>1709.7181029659082</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1687.1221299117801</c:v>
+                  <c:v>1706.5676595412967</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1686.0085942369142</c:v>
+                  <c:v>1703.1666891024681</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1685.1646273707279</c:v>
+                  <c:v>1699.7070178329891</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1684.6147841166214</c:v>
+                  <c:v>1696.4222165606698</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1684.4159751788936</c:v>
+                  <c:v>1693.5545182897536</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1684.6464062931789</c:v>
+                  <c:v>1691.3215248417596</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1685.3842571923612</c:v>
+                  <c:v>1689.8903506425297</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1686.6762442319032</c:v>
+                  <c:v>1689.3494662363858</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1688.3866689887257</c:v>
+                  <c:v>1689.5657670910662</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1689.202384059744</c:v>
+                  <c:v>1689.2024215313747</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12244,16 +12456,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25984,8 +26196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE156"/>
   <sheetViews>
-    <sheetView topLeftCell="J10" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:AE42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34339,10 +34551,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:BQ130"/>
+  <dimension ref="A1:BQ134"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34730,7 +34942,8 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>-58.205179707705952</v>
+        <f>G4-273.15</f>
+        <v>55.000817051530021</v>
       </c>
       <c r="C4">
         <v>42.770640332440799</v>
@@ -34743,6 +34956,9 @@
       </c>
       <c r="F4">
         <v>576</v>
+      </c>
+      <c r="G4">
+        <v>328.15081705153</v>
       </c>
     </row>
     <row r="5" spans="1:60" x14ac:dyDescent="0.25">
@@ -34750,7 +34966,8 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>58.626986457407497</v>
+        <f t="shared" ref="B5:B65" si="0">G5-273.15</f>
+        <v>55.171820214391005</v>
       </c>
       <c r="C5">
         <v>44.906728683645397</v>
@@ -34763,6 +34980,9 @@
       </c>
       <c r="F5">
         <v>576</v>
+      </c>
+      <c r="G5">
+        <v>328.32182021439098</v>
       </c>
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.25">
@@ -34770,7 +34990,8 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>83.081676228344463</v>
+        <f t="shared" si="0"/>
+        <v>72.220900034904048</v>
       </c>
       <c r="C6">
         <v>45.434369618188803</v>
@@ -34783,6 +35004,9 @@
       </c>
       <c r="F6">
         <v>577.34577656750002</v>
+      </c>
+      <c r="G6">
+        <v>345.37090003490403</v>
       </c>
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.25">
@@ -34790,7 +35014,8 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>108.71960984021428</v>
+        <f t="shared" si="0"/>
+        <v>93.934105640650046</v>
       </c>
       <c r="C7">
         <v>45.695753646172797</v>
@@ -34803,6 +35028,9 @@
       </c>
       <c r="F7">
         <v>578.69155313500096</v>
+      </c>
+      <c r="G7">
+        <v>367.08410564065002</v>
       </c>
     </row>
     <row r="8" spans="1:60" x14ac:dyDescent="0.25">
@@ -34810,7 +35038,8 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>122.88854920715096</v>
+        <f t="shared" si="0"/>
+        <v>112.53271219730402</v>
       </c>
       <c r="C8">
         <v>45.8871277101563</v>
@@ -34823,6 +35052,9 @@
       </c>
       <c r="F8">
         <v>580.03732970250098</v>
+      </c>
+      <c r="G8">
+        <v>385.682712197304</v>
       </c>
     </row>
     <row r="9" spans="1:60" x14ac:dyDescent="0.25">
@@ -34830,7 +35062,8 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>128.84751611799004</v>
+        <f t="shared" si="0"/>
+        <v>125.59896901100905</v>
       </c>
       <c r="C9">
         <v>46.054600563038697</v>
@@ -34843,6 +35076,9 @@
       </c>
       <c r="F9">
         <v>581.38310627000101</v>
+      </c>
+      <c r="G9">
+        <v>398.74896901100902</v>
       </c>
     </row>
     <row r="10" spans="1:60" x14ac:dyDescent="0.25">
@@ -34850,7 +35086,8 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>132.0132655784488</v>
+        <f t="shared" si="0"/>
+        <v>132.81194061636904</v>
       </c>
       <c r="C10">
         <v>46.227242331734502</v>
@@ -34863,6 +35100,9 @@
       </c>
       <c r="F10">
         <v>582.72888283750103</v>
+      </c>
+      <c r="G10">
+        <v>405.96194061636902</v>
       </c>
     </row>
     <row r="11" spans="1:60" x14ac:dyDescent="0.25">
@@ -34870,7 +35110,8 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>135.05399541407826</v>
+        <f t="shared" si="0"/>
+        <v>132.93185184747</v>
       </c>
       <c r="C11">
         <v>46.477138698471101</v>
@@ -34883,6 +35124,9 @@
       </c>
       <c r="F11">
         <v>584.07465940500197</v>
+      </c>
+      <c r="G11">
+        <v>406.08185184746998</v>
       </c>
     </row>
     <row r="12" spans="1:60" x14ac:dyDescent="0.25">
@@ -34890,7 +35134,8 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>138.50626849979164</v>
+        <f t="shared" si="0"/>
+        <v>124.766830688715</v>
       </c>
       <c r="C12">
         <v>47.285981535291597</v>
@@ -34903,6 +35148,9 @@
       </c>
       <c r="F12">
         <v>585.42043597250199</v>
+      </c>
+      <c r="G12">
+        <v>397.91683068871498</v>
       </c>
     </row>
     <row r="13" spans="1:60" x14ac:dyDescent="0.25">
@@ -34910,7 +35158,8 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>141.76056587547066</v>
+        <f t="shared" si="0"/>
+        <v>110.63953811526301</v>
       </c>
       <c r="C13">
         <v>52.222918010638701</v>
@@ -34923,6 +35172,9 @@
       </c>
       <c r="F13">
         <v>586.76621254000202</v>
+      </c>
+      <c r="G13">
+        <v>383.78953811526299</v>
       </c>
     </row>
     <row r="14" spans="1:60" x14ac:dyDescent="0.25">
@@ -34930,7 +35182,8 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>151.79324352592232</v>
+        <f t="shared" si="0"/>
+        <v>152.36483076810805</v>
       </c>
       <c r="C14">
         <v>52.7741896013844</v>
@@ -34943,6 +35196,9 @@
       </c>
       <c r="F14">
         <v>588.11198910750204</v>
+      </c>
+      <c r="G14">
+        <v>425.51483076810803</v>
       </c>
     </row>
     <row r="15" spans="1:60" x14ac:dyDescent="0.25">
@@ -34950,7 +35206,8 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>153.29639853388073</v>
+        <f t="shared" si="0"/>
+        <v>165.50789041668202</v>
       </c>
       <c r="C15">
         <v>53.037096580507601</v>
@@ -34963,6 +35220,9 @@
       </c>
       <c r="F15">
         <v>589.45776567500297</v>
+      </c>
+      <c r="G15">
+        <v>438.65789041668199</v>
       </c>
     </row>
     <row r="16" spans="1:60" x14ac:dyDescent="0.25">
@@ -34970,7 +35230,8 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>153.63409274667504</v>
+        <f t="shared" si="0"/>
+        <v>168.40496352911003</v>
       </c>
       <c r="C16">
         <v>53.184739001984099</v>
@@ -34983,6 +35244,9 @@
       </c>
       <c r="F16">
         <v>590.803542242503</v>
+      </c>
+      <c r="G16">
+        <v>441.55496352911001</v>
       </c>
     </row>
     <row r="17" spans="1:69" x14ac:dyDescent="0.25">
@@ -34990,7 +35254,8 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>153.80268969982865</v>
+        <f t="shared" si="0"/>
+        <v>169.20902319103504</v>
       </c>
       <c r="C17">
         <v>53.285389833478398</v>
@@ -35003,6 +35268,9 @@
       </c>
       <c r="F17">
         <v>592.14931881000302</v>
+      </c>
+      <c r="G17">
+        <v>442.35902319103502</v>
       </c>
     </row>
     <row r="18" spans="1:69" x14ac:dyDescent="0.25">
@@ -35010,7 +35278,8 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>153.93933036774399</v>
+        <f t="shared" si="0"/>
+        <v>169.54984563440104</v>
       </c>
       <c r="C18">
         <v>53.365235835489202</v>
@@ -35023,6 +35292,9 @@
       </c>
       <c r="F18">
         <v>593.49509537750305</v>
+      </c>
+      <c r="G18">
+        <v>442.69984563440102</v>
       </c>
     </row>
     <row r="19" spans="1:69" x14ac:dyDescent="0.25">
@@ -35030,7 +35302,8 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>154.06756715327504</v>
+        <f t="shared" si="0"/>
+        <v>169.736493049562</v>
       </c>
       <c r="C19">
         <v>53.433699775111101</v>
@@ -35043,6 +35316,9 @@
       </c>
       <c r="F19">
         <v>594.84087194500398</v>
+      </c>
+      <c r="G19">
+        <v>442.88649304956198</v>
       </c>
     </row>
     <row r="20" spans="1:69" x14ac:dyDescent="0.25">
@@ -35050,7 +35326,8 @@
         <v>17</v>
       </c>
       <c r="B20">
-        <v>154.19370771795514</v>
+        <f t="shared" si="0"/>
+        <v>169.839338867366</v>
       </c>
       <c r="C20">
         <v>53.493682430376502</v>
@@ -35063,6 +35340,9 @@
       </c>
       <c r="F20">
         <v>596.18664851250401</v>
+      </c>
+      <c r="G20">
+        <v>442.98933886736597</v>
       </c>
     </row>
     <row r="21" spans="1:69" x14ac:dyDescent="0.25">
@@ -35070,7 +35350,8 @@
         <v>18</v>
       </c>
       <c r="B21">
-        <v>154.32059557586911</v>
+        <f t="shared" si="0"/>
+        <v>169.87773819863804</v>
       </c>
       <c r="C21">
         <v>53.5451659713354</v>
@@ -35083,6 +35364,9 @@
       </c>
       <c r="F21">
         <v>597.53242508000403</v>
+      </c>
+      <c r="G21">
+        <v>443.02773819863802</v>
       </c>
     </row>
     <row r="22" spans="1:69" x14ac:dyDescent="0.25">
@@ -35090,7 +35374,8 @@
         <v>19</v>
       </c>
       <c r="B22">
-        <v>154.45014329105618</v>
+        <f t="shared" si="0"/>
+        <v>169.85121863186401</v>
       </c>
       <c r="C22">
         <v>53.586199327556201</v>
@@ -35103,6 +35388,9 @@
       </c>
       <c r="F22">
         <v>598.87820164750406</v>
+      </c>
+      <c r="G22">
+        <v>443.00121863186399</v>
       </c>
     </row>
     <row r="23" spans="1:69" x14ac:dyDescent="0.25">
@@ -35110,7 +35398,8 @@
         <v>20</v>
       </c>
       <c r="B23">
-        <v>154.58409243673088</v>
+        <f t="shared" si="0"/>
+        <v>169.73703181594601</v>
       </c>
       <c r="C23">
         <v>53.611292230714497</v>
@@ -35123,6 +35412,9 @@
       </c>
       <c r="F23">
         <v>600.22397821500499</v>
+      </c>
+      <c r="G23">
+        <v>442.88703181594599</v>
       </c>
     </row>
     <row r="24" spans="1:69" x14ac:dyDescent="0.25">
@@ -35130,7 +35422,8 @@
         <v>21</v>
       </c>
       <c r="B24">
-        <v>154.72448856979611</v>
+        <f t="shared" si="0"/>
+        <v>169.46226681619902</v>
       </c>
       <c r="C24">
         <v>53.595120146984797</v>
@@ -35143,6 +35436,9 @@
       </c>
       <c r="F24">
         <v>601.56975478250502</v>
+      </c>
+      <c r="G24">
+        <v>442.612266816199</v>
       </c>
       <c r="H24">
         <v>0.57599999999999996</v>
@@ -35336,7 +35632,8 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>154.87401054650547</v>
+        <f t="shared" si="0"/>
+        <v>168.77262965440804</v>
       </c>
       <c r="C25">
         <v>53.267428832761397</v>
@@ -35349,253 +35646,256 @@
       </c>
       <c r="F25">
         <v>602.91553135000504</v>
+      </c>
+      <c r="G25">
+        <v>441.92262965440801</v>
       </c>
       <c r="H25">
         <f>H24*1000</f>
         <v>576</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:BQ25" si="0">I24*1000</f>
+        <f t="shared" ref="I25:BQ25" si="1">I24*1000</f>
         <v>577.27419354838707</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>578.54838709677404</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>579.822580645161</v>
       </c>
       <c r="L25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>581.09677419354796</v>
       </c>
       <c r="M25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>582.37096774193492</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>583.6451612903229</v>
       </c>
       <c r="O25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>584.91935483871009</v>
       </c>
       <c r="P25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>586.19354838709705</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>587.46774193548401</v>
       </c>
       <c r="R25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>588.74193548387098</v>
       </c>
       <c r="S25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>590.01612903225794</v>
       </c>
       <c r="T25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>591.29032258064501</v>
       </c>
       <c r="U25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>592.56451612903209</v>
       </c>
       <c r="V25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>593.83870967741905</v>
       </c>
       <c r="W25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>595.11290322580601</v>
       </c>
       <c r="X25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>596.38709677419297</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>597.66129032258095</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>598.93548387096791</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>600.2096774193551</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>601.48387096774206</v>
       </c>
       <c r="AC25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>602.75806451612902</v>
       </c>
       <c r="AD25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>604.03225806451599</v>
       </c>
       <c r="AE25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>605.30645161290295</v>
       </c>
       <c r="AF25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>606.58064516128991</v>
       </c>
       <c r="AG25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>607.8548387096771</v>
       </c>
       <c r="AH25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>609.12903225806406</v>
       </c>
       <c r="AI25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>610.40322580645102</v>
       </c>
       <c r="AJ25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>611.677419354839</v>
       </c>
       <c r="AK25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>612.95161290322596</v>
       </c>
       <c r="AL25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>614.22580645161293</v>
       </c>
       <c r="AM25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>615.5</v>
       </c>
       <c r="AN25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>616.77419354838707</v>
       </c>
       <c r="AO25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>618.04838709677404</v>
       </c>
       <c r="AP25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>619.322580645161</v>
       </c>
       <c r="AQ25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>620.59677419354796</v>
       </c>
       <c r="AR25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>621.87096774193492</v>
       </c>
       <c r="AS25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>623.14516129032199</v>
       </c>
       <c r="AT25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>624.41935483870907</v>
       </c>
       <c r="AU25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>625.69354838709705</v>
       </c>
       <c r="AV25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>626.96774193548401</v>
       </c>
       <c r="AW25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>628.24193548387098</v>
       </c>
       <c r="AX25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>629.51612903225794</v>
       </c>
       <c r="AY25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>630.79032258064501</v>
       </c>
       <c r="AZ25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>632.06451612903197</v>
       </c>
       <c r="BA25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>633.33870967741905</v>
       </c>
       <c r="BB25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>634.61290322580601</v>
       </c>
       <c r="BC25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>635.88709677419297</v>
       </c>
       <c r="BD25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>637.16129032257993</v>
       </c>
       <c r="BE25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>638.435483870967</v>
       </c>
       <c r="BF25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>639.70967741935499</v>
       </c>
       <c r="BG25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>640.98387096774206</v>
       </c>
       <c r="BH25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>642.25806451612902</v>
       </c>
       <c r="BI25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>643.53225806451599</v>
       </c>
       <c r="BJ25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>644.80645161290295</v>
       </c>
       <c r="BK25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>646.08064516129002</v>
       </c>
       <c r="BL25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>647.35483870967698</v>
       </c>
       <c r="BM25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>648.62903225806406</v>
       </c>
       <c r="BN25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>649.90322580645102</v>
       </c>
       <c r="BO25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>651.17741935483798</v>
       </c>
       <c r="BP25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>652.45161290322596</v>
       </c>
       <c r="BQ25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>655</v>
       </c>
     </row>
@@ -35604,7 +35904,8 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <v>155.05002343505623</v>
+        <f t="shared" si="0"/>
+        <v>176.87378360182004</v>
       </c>
       <c r="C26">
         <v>53.365305779651798</v>
@@ -35617,6 +35918,9 @@
       </c>
       <c r="F26">
         <v>604.26130791750495</v>
+      </c>
+      <c r="G26">
+        <v>450.02378360182001</v>
       </c>
       <c r="H26">
         <v>576</v>
@@ -35810,7 +36114,8 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>155.22905082851651</v>
+        <f t="shared" si="0"/>
+        <v>177.49559807628401</v>
       </c>
       <c r="C27">
         <v>53.458887326907899</v>
@@ -35823,6 +36128,9 @@
       </c>
       <c r="F27">
         <v>605.607084485006</v>
+      </c>
+      <c r="G27">
+        <v>450.64559807628399</v>
       </c>
     </row>
     <row r="28" spans="1:69" x14ac:dyDescent="0.25">
@@ -35830,7 +36138,8 @@
         <v>25</v>
       </c>
       <c r="B28">
-        <v>155.42475299388173</v>
+        <f t="shared" si="0"/>
+        <v>176.85188388675505</v>
       </c>
       <c r="C28">
         <v>53.550750035862102</v>
@@ -35843,6 +36152,9 @@
       </c>
       <c r="F28">
         <v>606.95286105250602</v>
+      </c>
+      <c r="G28">
+        <v>450.00188388675502</v>
       </c>
     </row>
     <row r="29" spans="1:69" x14ac:dyDescent="0.25">
@@ -35850,7 +36162,8 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <v>155.64350092262032</v>
+        <f t="shared" si="0"/>
+        <v>175.96158978939104</v>
       </c>
       <c r="C29">
         <v>53.642366339583504</v>
@@ -35863,6 +36176,9 @@
       </c>
       <c r="F29">
         <v>608.29863762000605</v>
+      </c>
+      <c r="G29">
+        <v>449.11158978939102</v>
       </c>
     </row>
     <row r="30" spans="1:69" x14ac:dyDescent="0.25">
@@ -35870,7 +36186,8 @@
         <v>27</v>
       </c>
       <c r="B30">
-        <v>155.89207091778519</v>
+        <f t="shared" si="0"/>
+        <v>174.99488827437204</v>
       </c>
       <c r="C30">
         <v>53.734252450157399</v>
@@ -35883,6 +36200,9 @@
       </c>
       <c r="F30">
         <v>609.64441418750596</v>
+      </c>
+      <c r="G30">
+        <v>448.14488827437202</v>
       </c>
     </row>
     <row r="31" spans="1:69" x14ac:dyDescent="0.25">
@@ -35890,7 +36210,8 @@
         <v>28</v>
       </c>
       <c r="B31">
-        <v>156.17892385870221</v>
+        <f t="shared" si="0"/>
+        <v>174.00019245445702</v>
       </c>
       <c r="C31">
         <v>53.826807556226598</v>
@@ -35903,6 +36224,9 @@
       </c>
       <c r="F31">
         <v>610.99019075500701</v>
+      </c>
+      <c r="G31">
+        <v>447.150192454457</v>
       </c>
     </row>
     <row r="32" spans="1:69" x14ac:dyDescent="0.25">
@@ -35910,7 +36234,8 @@
         <v>29</v>
       </c>
       <c r="B32">
-        <v>156.51470550745728</v>
+        <f t="shared" si="0"/>
+        <v>173.01106522828303</v>
       </c>
       <c r="C32">
         <v>53.920447504538302</v>
@@ -35924,13 +36249,17 @@
       <c r="F32">
         <v>612.33596732250703</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>446.16106522828301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
       <c r="B33">
-        <v>156.9126138225198</v>
+        <f t="shared" si="0"/>
+        <v>172.05951786637303</v>
       </c>
       <c r="C33">
         <v>54.015555486012403</v>
@@ -35944,13 +36273,17 @@
       <c r="F33">
         <v>613.68174389000706</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>445.20951786637301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
       <c r="B34">
-        <v>157.38863327950241</v>
+        <f t="shared" si="0"/>
+        <v>171.17544264942404</v>
       </c>
       <c r="C34">
         <v>54.112629436428101</v>
@@ -35964,13 +36297,17 @@
       <c r="F34">
         <v>615.02752045750697</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>444.32544264942402</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
       <c r="B35">
-        <v>157.9614398762584</v>
+        <f t="shared" si="0"/>
+        <v>170.38425194323105</v>
       </c>
       <c r="C35">
         <v>54.212261052956897</v>
@@ -35984,13 +36321,17 @@
       <c r="F35">
         <v>616.37329702500801</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>443.53425194323103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
       <c r="B36">
-        <v>158.65193249136212</v>
+        <f t="shared" si="0"/>
+        <v>169.70505134612301</v>
       </c>
       <c r="C36">
         <v>54.315430223097003</v>
@@ -36004,13 +36345,17 @@
       <c r="F36">
         <v>617.71907359250804</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>442.85505134612299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
       <c r="B37">
-        <v>159.48194095343354</v>
+        <f t="shared" si="0"/>
+        <v>169.149723751843</v>
       </c>
       <c r="C37">
         <v>54.422870035450302</v>
@@ -36024,13 +36369,17 @@
       <c r="F37">
         <v>619.06485016000795</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>442.29972375184298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
       <c r="B38">
-        <v>160.47199049443009</v>
+        <f t="shared" si="0"/>
+        <v>168.72308412790301</v>
       </c>
       <c r="C38">
         <v>54.535894156153603</v>
@@ -36044,13 +36393,17 @@
       <c r="F38">
         <v>620.41062672750797</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>441.87308412790298</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
       <c r="B39">
-        <v>161.63801492601635</v>
+        <f t="shared" si="0"/>
+        <v>168.42376068830504</v>
       </c>
       <c r="C39">
         <v>54.6564934271765</v>
@@ -36064,13 +36417,17 @@
       <c r="F39">
         <v>621.75640329500902</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>441.57376068830501</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
       <c r="B40">
-        <v>162.98725285977127</v>
+        <f t="shared" si="0"/>
+        <v>168.24555567503</v>
       </c>
       <c r="C40">
         <v>54.786753279440603</v>
@@ -36084,13 +36441,17 @@
       <c r="F40">
         <v>623.10217986250905</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>441.39555567502998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
       <c r="B41">
-        <v>164.51408059746029</v>
+        <f t="shared" si="0"/>
+        <v>168.1789244771</v>
       </c>
       <c r="C41">
         <v>54.928499217312897</v>
@@ -36104,13 +36465,17 @@
       <c r="F41">
         <v>624.44795643000896</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>441.32892447709997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
       <c r="B42">
-        <v>166.19709262102845</v>
+        <f t="shared" si="0"/>
+        <v>168.212406551838</v>
       </c>
       <c r="C42">
         <v>55.085919669328597</v>
@@ -36124,13 +36489,17 @@
       <c r="F42">
         <v>625.79373299750898</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>441.36240655183798</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
       <c r="B43">
-        <v>167.99874694496395</v>
+        <f t="shared" si="0"/>
+        <v>168.33396307230004</v>
       </c>
       <c r="C43">
         <v>55.262767148063098</v>
@@ -36144,13 +36513,17 @@
       <c r="F43">
         <v>627.13950956501003</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>441.48396307230001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
       <c r="B44">
-        <v>169.86855694502594</v>
+        <f t="shared" si="0"/>
+        <v>168.53216270208401</v>
       </c>
       <c r="C44">
         <v>55.464027048942299</v>
@@ -36164,13 +36537,17 @@
       <c r="F44">
         <v>628.48528613251005</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>441.68216270208399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
       <c r="B45">
-        <v>171.74947501569989</v>
+        <f t="shared" si="0"/>
+        <v>168.797297275066</v>
       </c>
       <c r="C45">
         <v>55.695565995082703</v>
@@ -36184,13 +36561,17 @@
       <c r="F45">
         <v>629.83106270000997</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>441.94729727506598</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
       <c r="B46">
-        <v>173.58582147806885</v>
+        <f t="shared" si="0"/>
+        <v>169.12240478247401</v>
       </c>
       <c r="C46">
         <v>55.963697502665099</v>
@@ -36204,13 +36585,17 @@
       <c r="F46">
         <v>631.17683926750999</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>442.27240478247398</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
       <c r="B47">
-        <v>175.33059285432103</v>
+        <f t="shared" si="0"/>
+        <v>169.50424374491001</v>
       </c>
       <c r="C47">
         <v>56.277528443496102</v>
@@ -36224,13 +36609,17 @@
       <c r="F47">
         <v>632.52261583501104</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>442.65424374490999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
       <c r="B48">
-        <v>176.95013561695816</v>
+        <f t="shared" si="0"/>
+        <v>169.94396959841305</v>
       </c>
       <c r="C48">
         <v>56.642283785163599</v>
@@ -36244,13 +36633,17 @@
       <c r="F48">
         <v>633.86839240251095</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>443.09396959841303</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
       <c r="B49">
-        <v>178.42553944736721</v>
+        <f t="shared" si="0"/>
+        <v>170.44754781425002</v>
       </c>
       <c r="C49">
         <v>57.067212727468302</v>
@@ -36264,13 +36657,17 @@
       <c r="F49">
         <v>635.21416897001097</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>443.59754781424999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="B50">
-        <v>179.75121231228115</v>
+        <f t="shared" si="0"/>
+        <v>171.02559791356305</v>
       </c>
       <c r="C50">
         <v>57.559184555381201</v>
@@ -36284,13 +36681,17 @@
       <c r="F50">
         <v>636.559945537511</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>444.17559791356302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
       <c r="B51">
-        <v>180.93176463097336</v>
+        <f t="shared" si="0"/>
+        <v>171.69255943447405</v>
       </c>
       <c r="C51">
         <v>58.121686948638697</v>
@@ -36304,13 +36705,17 @@
       <c r="F51">
         <v>637.90572210501205</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>444.84255943447403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
       <c r="B52">
-        <v>181.97841213494542</v>
+        <f t="shared" si="0"/>
+        <v>172.464942342043</v>
       </c>
       <c r="C52">
         <v>58.753885163261202</v>
@@ -36324,13 +36729,17 @@
       <c r="F52">
         <v>639.25149867251196</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>445.61494234204298</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
       <c r="B53">
-        <v>182.90577137321236</v>
+        <f t="shared" si="0"/>
+        <v>173.35866351276604</v>
       </c>
       <c r="C53">
         <v>59.449971212343797</v>
@@ -36344,13 +36753,17 @@
       <c r="F53">
         <v>640.59727524001198</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>446.50866351276602</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
       <c r="B54">
-        <v>183.72949117273095</v>
+        <f t="shared" si="0"/>
+        <v>174.38537116944804</v>
       </c>
       <c r="C54">
         <v>60.197818620175902</v>
@@ -36364,13 +36777,17 @@
       <c r="F54">
         <v>641.94305180751201</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>447.53537116944801</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
       <c r="B55">
-        <v>184.46491637676957</v>
+        <f t="shared" si="0"/>
+        <v>175.54850345701004</v>
       </c>
       <c r="C55">
         <v>60.9803601345698</v>
@@ -36384,13 +36801,17 @@
       <c r="F55">
         <v>643.28882837501305</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>448.69850345701002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
       <c r="B56">
-        <v>185.12687252312901</v>
+        <f t="shared" si="0"/>
+        <v>176.84007284641302</v>
       </c>
       <c r="C56">
         <v>61.777024756998799</v>
@@ -36404,13 +36825,17 @@
       <c r="F56">
         <v>644.63460494251296</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>449.990072846413</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
       <c r="B57">
-        <v>185.73079311698677</v>
+        <f t="shared" si="0"/>
+        <v>178.23973857462403</v>
       </c>
       <c r="C57">
         <v>62.567025428430597</v>
@@ -36424,13 +36849,17 @@
       <c r="F57">
         <v>645.98038151001299</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>451.389738574624</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58">
-        <v>186.29528449326756</v>
+        <f t="shared" si="0"/>
+        <v>179.71747495085003</v>
       </c>
       <c r="C58">
         <v>63.333913811673902</v>
@@ -36444,13 +36873,17 @@
       <c r="F58">
         <v>647.32615807751301</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>452.86747495085001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
       <c r="B59">
-        <v>186.8454189732671</v>
+        <f t="shared" si="0"/>
+        <v>181.23980717212004</v>
       </c>
       <c r="C59">
         <v>64.072470274829399</v>
@@ -36464,13 +36897,17 @@
       <c r="F59">
         <v>648.67193464501395</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>454.38980717212002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
       <c r="B60">
-        <v>187.41488174945118</v>
+        <f t="shared" si="0"/>
+        <v>182.77838464677302</v>
       </c>
       <c r="C60">
         <v>64.801247754856703</v>
@@ -36484,13 +36921,17 @@
       <c r="F60">
         <v>650.01771121251397</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>455.928384646773</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
       <c r="B61">
-        <v>188.04459662586453</v>
+        <f t="shared" si="0"/>
+        <v>184.318712508678</v>
       </c>
       <c r="C61">
         <v>65.592700236618299</v>
@@ -36504,13 +36945,17 @@
       <c r="F61">
         <v>651.363487780014</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>457.46871250867798</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
       <c r="B62">
-        <v>188.78096544593575</v>
+        <f t="shared" si="0"/>
+        <v>185.86896171271803</v>
       </c>
       <c r="C62">
         <v>66.6781824811154</v>
@@ -36524,13 +36969,17 @@
       <c r="F62">
         <v>652.70926434751402</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>459.01896171271801</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
       <c r="B63">
-        <v>189.68890772610905</v>
+        <f t="shared" si="0"/>
+        <v>187.47742044776703</v>
       </c>
       <c r="C63">
         <v>69.045257790581402</v>
@@ -36544,13 +36993,17 @@
       <c r="F63">
         <v>654.05504091501496</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>460.62742044776701</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
       <c r="B64">
-        <v>190.95411316901448</v>
+        <f t="shared" si="0"/>
+        <v>189.33045492917302</v>
       </c>
       <c r="C64">
         <v>78.857783433238893</v>
@@ -36560,6 +37013,9 @@
       </c>
       <c r="F64">
         <v>655.40081748251498</v>
+      </c>
+      <c r="G64">
+        <v>462.48045492917299</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -36567,7 +37023,8 @@
         <v>62</v>
       </c>
       <c r="B65">
-        <v>193.82552409023049</v>
+        <f t="shared" si="0"/>
+        <v>192.67918667793305</v>
       </c>
       <c r="C65">
         <v>118.513084445343</v>
@@ -36577,6 +37034,9 @@
       </c>
       <c r="F65">
         <v>655.40081748251498</v>
+      </c>
+      <c r="G65">
+        <v>465.82918667793302</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -36624,7 +37084,7 @@
         <v>2.4412993835254299E-5</v>
       </c>
       <c r="G69" s="9">
-        <v>376.20000126596278</v>
+        <v>376.19999867213244</v>
       </c>
       <c r="H69" s="9">
         <v>0</v>
@@ -36647,10 +37107,10 @@
         <v>1689.19270119726</v>
       </c>
       <c r="G70" s="9">
-        <v>867.9917455829675</v>
+        <v>909.85364381938552</v>
       </c>
       <c r="H70" s="9">
-        <v>1689.2000056843815</v>
+        <v>1689.1999940376559</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -36670,10 +37130,10 @@
         <v>1686.67064477299</v>
       </c>
       <c r="G71" s="9">
-        <v>722.82649187318975</v>
+        <v>811.11426126007427</v>
       </c>
       <c r="H71" s="9">
-        <v>2180.9917500013862</v>
+        <v>2222.8536391849088</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -36693,10 +37153,10 @@
         <v>1684.73410321713</v>
       </c>
       <c r="G72" s="9">
-        <v>628.99995090415359</v>
+        <v>712.45688666045044</v>
       </c>
       <c r="H72" s="9">
-        <v>2035.8264962916085</v>
+        <v>2124.1142566255976</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -36716,10 +37176,10 @@
         <v>1683.2382493499999</v>
       </c>
       <c r="G73" s="9">
-        <v>589.31788134235785</v>
+        <v>643.48412279106265</v>
       </c>
       <c r="H73" s="9">
-        <v>1941.9999553225723</v>
+        <v>2025.4568820259738</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -36739,10 +37199,10 @@
         <v>1681.94274595722</v>
       </c>
       <c r="G74" s="9">
-        <v>567.86493934369014</v>
+        <v>614.88214315558139</v>
       </c>
       <c r="H74" s="9">
-        <v>1902.3178857607766</v>
+        <v>1956.484118156586</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -36762,10 +37222,10 @@
         <v>1680.5871066960799</v>
       </c>
       <c r="G75" s="9">
-        <v>545.68109523684029</v>
+        <v>636.11191126241943</v>
       </c>
       <c r="H75" s="9">
-        <v>1880.8649437621089</v>
+        <v>1927.8821385211047</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -36785,10 +37245,10 @@
         <v>1678.4811758027499</v>
       </c>
       <c r="G76" s="9">
-        <v>519.92449148269702</v>
+        <v>702.61492060264573</v>
       </c>
       <c r="H76" s="9">
-        <v>1858.681099655259</v>
+        <v>1949.1119066279427</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -36808,10 +37268,10 @@
         <v>1671.0790606069299</v>
       </c>
       <c r="G77" s="9">
-        <v>498.32001842727118</v>
+        <v>777.8852463783378</v>
       </c>
       <c r="H77" s="9">
-        <v>1832.9244959011157</v>
+        <v>2015.614915968169</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -36831,10 +37291,10 @@
         <v>1625.6623785813899</v>
       </c>
       <c r="G78" s="9">
-        <v>2051.006183820733</v>
+        <v>2089.2544696749046</v>
       </c>
       <c r="H78" s="9">
-        <v>1811.3200228456899</v>
+        <v>2090.8852417438611</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -36854,10 +37314,10 @@
         <v>1802.6683890167899</v>
       </c>
       <c r="G79" s="9">
-        <v>2055.5090818604285</v>
+        <v>2045.3642735460312</v>
       </c>
       <c r="H79" s="9">
-        <v>1746.0061882391517</v>
+        <v>1784.2544650404282</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -36877,10 +37337,10 @@
         <v>1807.4716047024001</v>
       </c>
       <c r="G80" s="9">
-        <v>2056.2079786147524</v>
+        <v>2048.9037162776849</v>
       </c>
       <c r="H80" s="9">
-        <v>1750.5090862788472</v>
+        <v>1740.3642689115545</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -36900,10 +37360,10 @@
         <v>1809.8832660636001</v>
       </c>
       <c r="G81" s="9">
-        <v>2056.4149139530045</v>
+        <v>2049.471863946123</v>
       </c>
       <c r="H81" s="9">
-        <v>1751.2079830331709</v>
+        <v>1743.9037116432082</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -36923,10 +37383,10 @@
         <v>1811.35128022252</v>
       </c>
       <c r="G82" s="9">
-        <v>2056.6640597590663</v>
+        <v>2049.2217861181471</v>
       </c>
       <c r="H82" s="9">
-        <v>1751.414918371423</v>
+        <v>1744.4718593116463</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -36946,10 +37406,10 @@
         <v>1812.4663006529299</v>
       </c>
       <c r="G83" s="9">
-        <v>2056.9776320920155</v>
+        <v>2049.0606017975488</v>
       </c>
       <c r="H83" s="9">
-        <v>1751.664064177485</v>
+        <v>1744.2217814836706</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -36969,10 +37429,10 @@
         <v>1813.4414373842101</v>
       </c>
       <c r="G84" s="9">
-        <v>2057.3343093744866</v>
+        <v>2049.0901984861221</v>
       </c>
       <c r="H84" s="9">
-        <v>1751.9776365104342</v>
+        <v>1744.0605971630719</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -36992,10 +37452,10 @@
         <v>1814.3961333165901</v>
       </c>
       <c r="G85" s="9">
-        <v>2057.7176956350113</v>
+        <v>2049.3124812701435</v>
       </c>
       <c r="H85" s="9">
-        <v>1752.3343137929053</v>
+        <v>1744.0901938516452</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -37015,10 +37475,10 @@
         <v>1815.3682371423599</v>
       </c>
       <c r="G86" s="9">
-        <v>2058.1175381047469</v>
+        <v>2049.7661798812583</v>
       </c>
       <c r="H86" s="9">
-        <v>1752.71770005343</v>
+        <v>1744.3124766356666</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -37038,10 +37498,10 @@
         <v>1816.38736661282</v>
       </c>
       <c r="G87" s="9">
-        <v>2058.5272313851319</v>
+        <v>2050.5828032628233</v>
       </c>
       <c r="H87" s="9">
-        <v>1753.1175425231654</v>
+        <v>1744.7661752467816</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -37061,10 +37521,10 @@
         <v>1817.51322226109</v>
       </c>
       <c r="G88" s="9">
-        <v>2058.9416942055032</v>
+        <v>2052.0927967116995</v>
       </c>
       <c r="H88" s="9">
-        <v>1753.5272358035509</v>
+        <v>1745.5827986283468</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -37084,10 +37544,10 @@
         <v>1819.0228865332999</v>
       </c>
       <c r="G89" s="9">
-        <v>2059.3557726827576</v>
+        <v>2055.1880157777414</v>
       </c>
       <c r="H89" s="9">
-        <v>1753.9416986239216</v>
+        <v>1747.0927920772228</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -37107,10 +37567,10 @@
         <v>1823.6094484259299</v>
       </c>
       <c r="G90" s="9">
-        <v>2161.8725261154887</v>
+        <v>2079.6829001349533</v>
       </c>
       <c r="H90" s="9">
-        <v>1754.355777101176</v>
+        <v>1750.1880111432645</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -37130,10 +37590,10 @@
         <v>1823.11083383306</v>
       </c>
       <c r="G91" s="9">
-        <v>2162.2685348627374</v>
+        <v>2089.6522125134493</v>
       </c>
       <c r="H91" s="9">
-        <v>1753.7725305339075</v>
+        <v>1671.5828955004765</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -37153,10 +37613,10 @@
         <v>1824.0303035187401</v>
       </c>
       <c r="G92" s="9">
-        <v>2162.6320508319604</v>
+        <v>2093.8347542120609</v>
       </c>
       <c r="H92" s="9">
-        <v>1754.1685392811562</v>
+        <v>1681.5522078789725</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -37176,10 +37636,10 @@
         <v>1824.8940923463699</v>
       </c>
       <c r="G93" s="9">
-        <v>2162.9619404110949</v>
+        <v>2097.0369538259174</v>
       </c>
       <c r="H93" s="9">
-        <v>1754.5320552503792</v>
+        <v>1685.7347495775841</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -37199,10 +37659,10 @@
         <v>1825.78968474417</v>
       </c>
       <c r="G94" s="9">
-        <v>2163.2447272041863</v>
+        <v>2100.2131034368695</v>
       </c>
       <c r="H94" s="9">
-        <v>1754.8619448295135</v>
+        <v>1688.9369491914406</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -37222,10 +37682,10 @@
         <v>1826.64311337494</v>
       </c>
       <c r="G95" s="9">
-        <v>2163.4599146675514</v>
+        <v>2103.4616496155077</v>
       </c>
       <c r="H95" s="9">
-        <v>1755.1447316226049</v>
+        <v>1692.1130988023929</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -37245,10 +37705,10 @@
         <v>1827.48962894791</v>
       </c>
       <c r="G96" s="9">
-        <v>2163.5790887565763</v>
+        <v>2106.7410073133951</v>
       </c>
       <c r="H96" s="9">
-        <v>1755.35991908597</v>
+        <v>1695.3616449810308</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -37268,10 +37728,10 @@
         <v>1828.33206244543</v>
       </c>
       <c r="G97" s="9">
-        <v>2163.5641461400651</v>
+        <v>2109.9837721712488</v>
       </c>
       <c r="H97" s="9">
-        <v>1755.4790931749951</v>
+        <v>1698.6410026789185</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -37291,10 +37751,10 @@
         <v>1829.1498138985801</v>
       </c>
       <c r="G98" s="9">
-        <v>2163.3655167382658</v>
+        <v>2113.1175366562934</v>
       </c>
       <c r="H98" s="9">
-        <v>1755.4641505584839</v>
+        <v>1701.883767536772</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -37314,10 +37774,10 @@
         <v>1829.94438480495</v>
       </c>
       <c r="G99" s="9">
-        <v>2162.9209523929394</v>
+        <v>2116.072703839036</v>
       </c>
       <c r="H99" s="9">
-        <v>1755.2655211566846</v>
+        <v>1705.0175320218166</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -37337,10 +37797,10 @@
         <v>1830.70714843421</v>
       </c>
       <c r="G100" s="9">
-        <v>2162.1555640906658</v>
+        <v>2118.7881680600103</v>
       </c>
       <c r="H100" s="9">
-        <v>1754.820956811358</v>
+        <v>1707.9726992045594</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -37360,10 +37820,10 @@
         <v>1831.44383287716</v>
       </c>
       <c r="G101" s="9">
-        <v>2160.9845294087968</v>
+        <v>2121.2160497266177</v>
       </c>
       <c r="H101" s="9">
-        <v>1754.0555685090844</v>
+        <v>1710.6881634255337</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -37383,10 +37843,10 @@
         <v>1832.07700851914</v>
       </c>
       <c r="G102" s="9">
-        <v>2159.3193346659336</v>
+        <v>2123.3246214328178</v>
       </c>
       <c r="H102" s="9">
-        <v>1752.8845338272154</v>
+        <v>1713.1160450921411</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -37406,10 +37866,10 @@
         <v>1832.6889456737199</v>
       </c>
       <c r="G103" s="9">
-        <v>2157.0787096583044</v>
+        <v>2125.0993461402313</v>
       </c>
       <c r="H103" s="9">
-        <v>1751.2193390843524</v>
+        <v>1715.224616798341</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -37429,10 +37889,10 @@
         <v>1833.27099962594</v>
       </c>
       <c r="G104" s="9">
-        <v>2154.204028405552</v>
+        <v>2126.5417820348771</v>
       </c>
       <c r="H104" s="9">
-        <v>1748.978714076723</v>
+        <v>1716.9993415057545</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -37452,10 +37912,10 @@
         <v>1833.69538440163</v>
       </c>
       <c r="G105" s="9">
-        <v>2150.6769076461283</v>
+        <v>2127.6669405904549</v>
       </c>
       <c r="H105" s="9">
-        <v>1746.1040328239708</v>
+        <v>1718.4417774004005</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -37475,10 +37935,10 @@
         <v>1833.9283134412899</v>
       </c>
       <c r="G106" s="9">
-        <v>2146.5343135290996</v>
+        <v>2128.499532554295</v>
       </c>
       <c r="H106" s="9">
-        <v>1742.5769120645468</v>
+        <v>1719.5669359559784</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -37498,10 +37958,10 @@
         <v>1834.23918064949</v>
       </c>
       <c r="G107" s="9">
-        <v>2141.8751890000103</v>
+        <v>2129.0696848081507</v>
       </c>
       <c r="H107" s="9">
-        <v>1738.4343179475184</v>
+        <v>1720.3995279198184</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -37521,10 +37981,10 @@
         <v>1834.31138354991</v>
       </c>
       <c r="G108" s="9">
-        <v>2136.8536352480724</v>
+        <v>2129.4085592256206</v>
       </c>
       <c r="H108" s="9">
-        <v>1733.7751934184289</v>
+        <v>1720.9696801736739</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -37544,10 +38004,10 @@
         <v>1834.22385659784</v>
       </c>
       <c r="G109" s="9">
-        <v>2131.6586199086041</v>
+        <v>2129.5439550814513</v>
       </c>
       <c r="H109" s="9">
-        <v>1728.7536396664909</v>
+        <v>1721.3085545911438</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -37567,10 +38027,10 @@
         <v>1833.93736706594</v>
       </c>
       <c r="G110" s="9">
-        <v>2126.4856340255246</v>
+        <v>2129.4961499048677</v>
       </c>
       <c r="H110" s="9">
-        <v>1723.5586243270227</v>
+        <v>1721.4439504469744</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -37590,10 +38050,10 @@
         <v>1833.42356782605</v>
       </c>
       <c r="G111" s="9">
-        <v>2121.5091542204245</v>
+        <v>2129.2740977783824</v>
       </c>
       <c r="H111" s="9">
-        <v>1718.3856384439432</v>
+        <v>1721.3961452703911</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -37613,10 +38073,10 @@
         <v>1832.8507522954301</v>
       </c>
       <c r="G112" s="9">
-        <v>2116.8639076771515</v>
+        <v>2128.8724620812809</v>
       </c>
       <c r="H112" s="9">
-        <v>1713.4091586388433</v>
+        <v>1721.1740931439058</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -37636,10 +38096,10 @@
         <v>1831.63049238688</v>
       </c>
       <c r="G113" s="9">
-        <v>2112.6377433430371</v>
+        <v>2128.2695938737802</v>
       </c>
       <c r="H113" s="9">
-        <v>1708.76391209557</v>
+        <v>1720.7724574468043</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -37659,10 +38119,10 @@
         <v>1830.6774215267201</v>
       </c>
       <c r="G114" s="9">
-        <v>2108.8745424564959</v>
+        <v>2127.4275086505199</v>
       </c>
       <c r="H114" s="9">
-        <v>1704.5377477614559</v>
+        <v>1720.1695892393034</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -37682,10 +38142,10 @@
         <v>1829.4897040455601</v>
       </c>
       <c r="G115" s="9">
-        <v>2105.582892299843</v>
+        <v>2126.2944122376734</v>
       </c>
       <c r="H115" s="9">
-        <v>1700.7745468749144</v>
+        <v>1719.3275040160433</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -37705,10 +38165,10 @@
         <v>1827.89625489421</v>
       </c>
       <c r="G116" s="9">
-        <v>2102.7463492180677</v>
+        <v>2124.8110057568747</v>
       </c>
       <c r="H116" s="9">
-        <v>1697.4828967182616</v>
+        <v>1718.1944076031969</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -37728,10 +38188,10 @@
         <v>1825.9853932389401</v>
       </c>
       <c r="G117" s="9">
-        <v>2100.3327451973105</v>
+        <v>2122.9214452876827</v>
       </c>
       <c r="H117" s="9">
-        <v>1694.6463536364865</v>
+        <v>1716.7110011223981</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -37751,10 +38211,10 @@
         <v>1823.9610357799399</v>
       </c>
       <c r="G118" s="9">
-        <v>2098.3017240356585</v>
+        <v>2120.5895308067616</v>
       </c>
       <c r="H118" s="9">
-        <v>1692.2327496157293</v>
+        <v>1714.8214406532059</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -37774,10 +38234,10 @@
         <v>1821.9267078276</v>
       </c>
       <c r="G119" s="9">
-        <v>2096.6109325394668</v>
+        <v>2117.8181076003848</v>
       </c>
       <c r="H119" s="9">
-        <v>1690.2017284540771</v>
+        <v>1712.4895261722847</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -37797,10 +38257,10 @@
         <v>1820.14156474071</v>
       </c>
       <c r="G120" s="9">
-        <v>2095.2221254933615</v>
+        <v>2114.6676641757736</v>
       </c>
       <c r="H120" s="9">
-        <v>1688.5109369578856</v>
+        <v>1709.7181029659082</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -37820,10 +38280,10 @@
         <v>1818.7042645689401</v>
       </c>
       <c r="G121" s="9">
-        <v>2094.1085898184956</v>
+        <v>2111.2666937369449</v>
       </c>
       <c r="H121" s="9">
-        <v>1687.1221299117801</v>
+        <v>1706.5676595412967</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -37843,10 +38303,10 @@
         <v>1817.67077654788</v>
       </c>
       <c r="G122" s="9">
-        <v>2093.2646229523093</v>
+        <v>2107.8070224674657</v>
       </c>
       <c r="H122" s="9">
-        <v>1686.0085942369142</v>
+        <v>1703.1666891024681</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -37866,10 +38326,10 @@
         <v>1817.0160045904399</v>
       </c>
       <c r="G123" s="9">
-        <v>2092.7147796982026</v>
+        <v>2104.5222211951464</v>
       </c>
       <c r="H123" s="9">
-        <v>1685.1646273707279</v>
+        <v>1699.7070178329891</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -37889,10 +38349,10 @@
         <v>1816.63066529141</v>
       </c>
       <c r="G124" s="9">
-        <v>2092.5159707604748</v>
+        <v>2101.6545229242302</v>
       </c>
       <c r="H124" s="9">
-        <v>1684.6147841166214</v>
+        <v>1696.4222165606698</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -37912,10 +38372,10 @@
         <v>1816.2300425866899</v>
       </c>
       <c r="G125" s="9">
-        <v>2092.7464018747601</v>
+        <v>2099.4215294762362</v>
       </c>
       <c r="H125" s="9">
-        <v>1684.4159751788936</v>
+        <v>1693.5545182897536</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -37935,10 +38395,10 @@
         <v>1815.0859054346099</v>
       </c>
       <c r="G126" s="9">
-        <v>2093.4842527739424</v>
+        <v>2097.9903552770065</v>
       </c>
       <c r="H126" s="9">
-        <v>1684.6464062931789</v>
+        <v>1691.3215248417596</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -37958,10 +38418,10 @@
         <v>1811.1431846381799</v>
       </c>
       <c r="G127" s="9">
-        <v>2094.7762398134846</v>
+        <v>2097.4494708708626</v>
       </c>
       <c r="H127" s="9">
-        <v>1685.3842571923612</v>
+        <v>1689.8903506425297</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -37981,13 +38441,13 @@
         <v>1795.2527030034601</v>
       </c>
       <c r="G128" s="9">
-        <v>2096.4866645703069</v>
+        <v>2097.665771725543</v>
       </c>
       <c r="H128" s="9">
-        <v>1686.6762442319032</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1689.3494662363858</v>
+      </c>
+    </row>
+    <row r="129" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>61</v>
       </c>
@@ -38004,13 +38464,13 @@
         <v>1708.7871303899301</v>
       </c>
       <c r="G129" s="9">
-        <v>2097.3023796413254</v>
+        <v>2097.3024261658516</v>
       </c>
       <c r="H129" s="9">
-        <v>1688.3866689887257</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1689.5657670910662</v>
+      </c>
+    </row>
+    <row r="130" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>62</v>
       </c>
@@ -38027,10 +38487,198 @@
         <v>1367.0960423517399</v>
       </c>
       <c r="G130" s="9">
-        <v>408.09999558158256</v>
+        <v>408.10000463447784</v>
       </c>
       <c r="H130" s="9">
-        <v>1689.202384059744</v>
+        <v>1689.2024215313747</v>
+      </c>
+    </row>
+    <row r="134" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1938</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1939</v>
+      </c>
+      <c r="E134" t="s">
+        <v>1940</v>
+      </c>
+      <c r="F134" t="s">
+        <v>1941</v>
+      </c>
+      <c r="G134" t="s">
+        <v>1942</v>
+      </c>
+      <c r="H134" t="s">
+        <v>1943</v>
+      </c>
+      <c r="I134" t="s">
+        <v>1944</v>
+      </c>
+      <c r="J134" t="s">
+        <v>1945</v>
+      </c>
+      <c r="K134" t="s">
+        <v>1946</v>
+      </c>
+      <c r="L134" t="s">
+        <v>1947</v>
+      </c>
+      <c r="M134" t="s">
+        <v>1948</v>
+      </c>
+      <c r="N134" t="s">
+        <v>1949</v>
+      </c>
+      <c r="O134" t="s">
+        <v>1950</v>
+      </c>
+      <c r="P134" t="s">
+        <v>1951</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>1952</v>
+      </c>
+      <c r="R134" t="s">
+        <v>1953</v>
+      </c>
+      <c r="S134" t="s">
+        <v>1954</v>
+      </c>
+      <c r="T134" t="s">
+        <v>1955</v>
+      </c>
+      <c r="U134" t="s">
+        <v>1956</v>
+      </c>
+      <c r="V134" t="s">
+        <v>1957</v>
+      </c>
+      <c r="W134" t="s">
+        <v>1958</v>
+      </c>
+      <c r="X134" t="s">
+        <v>1959</v>
+      </c>
+      <c r="Y134" t="s">
+        <v>1960</v>
+      </c>
+      <c r="Z134" t="s">
+        <v>1961</v>
+      </c>
+      <c r="AA134" t="s">
+        <v>1962</v>
+      </c>
+      <c r="AB134" t="s">
+        <v>1963</v>
+      </c>
+      <c r="AC134" t="s">
+        <v>1964</v>
+      </c>
+      <c r="AD134" t="s">
+        <v>1965</v>
+      </c>
+      <c r="AE134" t="s">
+        <v>1966</v>
+      </c>
+      <c r="AF134" t="s">
+        <v>1967</v>
+      </c>
+      <c r="AG134" t="s">
+        <v>1968</v>
+      </c>
+      <c r="AH134" t="s">
+        <v>1969</v>
+      </c>
+      <c r="AI134" t="s">
+        <v>1970</v>
+      </c>
+      <c r="AJ134" t="s">
+        <v>1971</v>
+      </c>
+      <c r="AK134" t="s">
+        <v>1972</v>
+      </c>
+      <c r="AL134" t="s">
+        <v>1973</v>
+      </c>
+      <c r="AM134" t="s">
+        <v>1974</v>
+      </c>
+      <c r="AN134" t="s">
+        <v>1975</v>
+      </c>
+      <c r="AO134" t="s">
+        <v>1976</v>
+      </c>
+      <c r="AP134" t="s">
+        <v>1977</v>
+      </c>
+      <c r="AQ134" t="s">
+        <v>1978</v>
+      </c>
+      <c r="AR134" t="s">
+        <v>1979</v>
+      </c>
+      <c r="AS134" t="s">
+        <v>1980</v>
+      </c>
+      <c r="AT134" t="s">
+        <v>1981</v>
+      </c>
+      <c r="AU134" t="s">
+        <v>1982</v>
+      </c>
+      <c r="AV134" t="s">
+        <v>1983</v>
+      </c>
+      <c r="AW134" t="s">
+        <v>1984</v>
+      </c>
+      <c r="AX134" t="s">
+        <v>1985</v>
+      </c>
+      <c r="AY134" t="s">
+        <v>1986</v>
+      </c>
+      <c r="AZ134" t="s">
+        <v>1987</v>
+      </c>
+      <c r="BA134" t="s">
+        <v>1988</v>
+      </c>
+      <c r="BB134" t="s">
+        <v>1989</v>
+      </c>
+      <c r="BC134" t="s">
+        <v>1990</v>
+      </c>
+      <c r="BD134" t="s">
+        <v>1991</v>
+      </c>
+      <c r="BE134" t="s">
+        <v>1992</v>
+      </c>
+      <c r="BF134" t="s">
+        <v>1993</v>
+      </c>
+      <c r="BG134" t="s">
+        <v>1994</v>
+      </c>
+      <c r="BH134" t="s">
+        <v>1995</v>
+      </c>
+      <c r="BI134" t="s">
+        <v>1996</v>
+      </c>
+      <c r="BJ134" t="s">
+        <v>1997</v>
       </c>
     </row>
   </sheetData>
@@ -55447,7 +56095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6AE07F-558D-498F-8CC3-8F33837DB2F7}">
   <dimension ref="A1:BJ95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="H34" sqref="H34:H95"/>
     </sheetView>
   </sheetViews>
@@ -62772,4 +63420,528 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB81913-7A8B-42A4-B25F-EAFCD1F43EAE}">
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.07671258533863E-2</v>
+      </c>
+      <c r="B4" s="10">
+        <v>9.3384205739410398E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.6574607379347299</v>
+      </c>
+      <c r="B5">
+        <v>5.9424893872710501E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3.4426830465593601</v>
+      </c>
+      <c r="B6">
+        <v>0.174695281352753</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5.4667405893600103</v>
+      </c>
+      <c r="B7">
+        <v>0.34571360914989002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6.2266211235405997</v>
+      </c>
+      <c r="B8">
+        <v>0.41924937337479601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6.1981321902628697</v>
+      </c>
+      <c r="B9">
+        <v>0.41685777885075997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5.8512691044709699</v>
+      </c>
+      <c r="B10">
+        <v>0.38333378154235598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5.3255983430424703</v>
+      </c>
+      <c r="B11">
+        <v>0.334021927260578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.6570053294513398</v>
+      </c>
+      <c r="B12">
+        <v>0.27438316506896798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3.9837831473887801</v>
+      </c>
+      <c r="B13">
+        <v>0.21820527233006801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8.0177229244424204</v>
+      </c>
+      <c r="B14">
+        <v>0.61232439913903502</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9.7550428669863294</v>
+      </c>
+      <c r="B15">
+        <v>0.81839090272356696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10.132111437136</v>
+      </c>
+      <c r="B16">
+        <v>0.86632148053567604</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10.204564452719399</v>
+      </c>
+      <c r="B17">
+        <v>0.87636024190456197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10.209709788680099</v>
+      </c>
+      <c r="B18">
+        <v>0.87790453373317801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10.1924355126925</v>
+      </c>
+      <c r="B19">
+        <v>0.87660604773763195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10.1624489112794</v>
+      </c>
+      <c r="B20">
+        <v>0.87369267916458204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10.122166246085801</v>
+      </c>
+      <c r="B21">
+        <v>0.86947219103670603</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10.0713366211994</v>
+      </c>
+      <c r="B22">
+        <v>0.86391634313803201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10.006777310622599</v>
+      </c>
+      <c r="B23">
+        <v>0.85662918609462801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9.9187478315357396</v>
+      </c>
+      <c r="B24">
+        <v>0.84639625573666399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9.7742866327066498</v>
+      </c>
+      <c r="B25">
+        <v>0.82912216090691804</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10.766932020582599</v>
+      </c>
+      <c r="B26">
+        <v>0.95711083718121404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10.7561173371093</v>
+      </c>
+      <c r="B27">
+        <v>0.95664897361568402</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10.577323199714399</v>
+      </c>
+      <c r="B28">
+        <v>0.93423576064418701</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>10.3720947331894</v>
+      </c>
+      <c r="B29">
+        <v>0.90854694364458899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10.1649386463257</v>
+      </c>
+      <c r="B30">
+        <v>0.88280614873528196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>9.9634390941665796</v>
+      </c>
+      <c r="B31">
+        <v>0.85798564813446998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>9.7724843873792295</v>
+      </c>
+      <c r="B32">
+        <v>0.83468570637010397</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9.5960236519352193</v>
+      </c>
+      <c r="B33">
+        <v>0.81336988832357404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9.4371611386099001</v>
+      </c>
+      <c r="B34">
+        <v>0.794384059750188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9.2981371659644392</v>
+      </c>
+      <c r="B35">
+        <v>0.77796086814279897</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>9.1804030304774695</v>
+      </c>
+      <c r="B36">
+        <v>0.76423521772329295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>9.0847716431836592</v>
+      </c>
+      <c r="B37">
+        <v>0.75326763466864999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>9.0116359241993802</v>
+      </c>
+      <c r="B38">
+        <v>0.74507421359082904</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>8.9611913422691405</v>
+      </c>
+      <c r="B39">
+        <v>0.73965553174675602</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>8.9336401052215795</v>
+      </c>
+      <c r="B40">
+        <v>0.73702234016834001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>8.9293474870083607</v>
+      </c>
+      <c r="B41">
+        <v>0.73721506329053299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>8.9489194258855704</v>
+      </c>
+      <c r="B42">
+        <v>0.74031388551566901</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>8.9931825068175399</v>
+      </c>
+      <c r="B43">
+        <v>0.74643739968653799</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>9.0630347574774408</v>
+      </c>
+      <c r="B44">
+        <v>0.75572582748042905</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>9.1591662050931397</v>
+      </c>
+      <c r="B45">
+        <v>0.76830796905355603</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>9.2816438147552507</v>
+      </c>
+      <c r="B46">
+        <v>0.78424986677316799</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>9.4294277645875795</v>
+      </c>
+      <c r="B47">
+        <v>0.80349159239858903</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>9.59992948051657</v>
+      </c>
+      <c r="B48">
+        <v>0.82578426314279696</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>9.7887695708256004</v>
+      </c>
+      <c r="B49">
+        <v>0.85064687735035505</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>9.9899059227474591</v>
+      </c>
+      <c r="B50">
+        <v>0.87736691073472595</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10.1961970471834</v>
+      </c>
+      <c r="B51">
+        <v>0.90505821022104205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>10.400315391965</v>
+      </c>
+      <c r="B52">
+        <v>0.93277132991208001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10.595763071600199</v>
+      </c>
+      <c r="B53">
+        <v>0.95962797443025305</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>10.7777001763281</v>
+      </c>
+      <c r="B54">
+        <v>0.98494078782967698</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>10.943387605723499</v>
+      </c>
+      <c r="B55">
+        <v>1.0082875458010701</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>11.0922019171086</v>
+      </c>
+      <c r="B56">
+        <v>1.0295281734059001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>11.2253431698147</v>
+      </c>
+      <c r="B57">
+        <v>1.0487766384847901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>11.3454210399013</v>
+      </c>
+      <c r="B58">
+        <v>1.06635145553225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>11.456071921422399</v>
+      </c>
+      <c r="B59">
+        <v>1.0827264533871499</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>11.561719834551299</v>
+      </c>
+      <c r="B60">
+        <v>1.09849911188584</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>11.6675692794102</v>
+      </c>
+      <c r="B61">
+        <v>1.1143907158548501</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>11.7801001474802</v>
+      </c>
+      <c r="B62">
+        <v>1.1313185686560401</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>11.909491072213999</v>
+      </c>
+      <c r="B63">
+        <v>1.1507471417180299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>12.084765597028399</v>
+      </c>
+      <c r="B64">
+        <v>1.17688317574219</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>12.471039205972501</v>
+      </c>
+      <c r="B65">
+        <v>1.23501973569825</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>